<commit_message>
finishing truss and base connections
</commit_message>
<xml_diff>
--- a/design exel sheet/hinged base connection.xlsx
+++ b/design exel sheet/hinged base connection.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmed\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmed\Desktop\Graduation-project\design exel sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="100">
   <si>
     <t>web length</t>
   </si>
@@ -554,44 +554,26 @@
     <t>total inertia , Ix , n direction</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">min stifferer plan length , </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color theme="3"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>L</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="13"/>
-        <color theme="3"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>st,min</t>
-    </r>
-  </si>
-  <si>
     <t>m direction stiffneres , flanges plan perpendicular stiffeners</t>
   </si>
   <si>
     <t>web plan perpendicular stiffeners , welded on flages</t>
+  </si>
+  <si>
+    <t>stiffeners weld area</t>
+  </si>
+  <si>
+    <t>stiffeners to plate weld thickness</t>
+  </si>
+  <si>
+    <t>min stifferer plan length ,bst,min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -657,14 +639,6 @@
     <font>
       <b/>
       <sz val="14"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -887,11 +861,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -903,13 +883,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -921,11 +895,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -939,6 +910,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -948,7 +922,415 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="2" builtinId="21"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="58">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF9C0006"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF9C0006"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF9C0006"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF9C0006"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF9C0006"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF9C0006"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF9C0006"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF9C0006"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF9C0006"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF9C0006"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF9C0006"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF9C0006"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF9C0006"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF9C0006"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF9C0006"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF9C0006"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF9C0006"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF9C0006"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF9C0006"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF9C0006"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF9C0006"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF9C0006"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF9C0006"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF9C0006"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1257,7 +1639,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>492488</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>162221</xdr:rowOff>
+      <xdr:rowOff>117397</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1550,10 +1932,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W34"/>
+  <dimension ref="A1:W35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V25" sqref="V25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1573,50 +1955,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="Q1" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="Q1" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
       <c r="T1" s="6"/>
-      <c r="U1" s="7" t="s">
+      <c r="U1" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
     </row>
     <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
       <c r="T2" s="6"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
-    </row>
-    <row r="3" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+    </row>
+    <row r="3" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1637,16 +2019,16 @@
         <v>15</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="R3" s="13">
+        <v>99</v>
+      </c>
+      <c r="R3" s="9">
         <f>IF((B7-L3)/2-L12&gt;0,(B7-L3)/2-L12,"no stiffeners required ")</f>
         <v>11.443809065191434</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="U3" s="8" t="s">
+      <c r="U3" s="7" t="s">
         <v>45</v>
       </c>
       <c r="V3" s="2">
@@ -1680,7 +2062,7 @@
       <c r="Q4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="R4" s="13">
+      <c r="R4" s="9">
         <f>IF(B19&gt;0, IF(B21, B21, _xlfn.CEILING.MATH(L3/3)), 0)</f>
         <v>20</v>
       </c>
@@ -1762,7 +2144,7 @@
       <c r="Q6" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="R6" s="13">
+      <c r="R6" s="9">
         <f>MAX(B20,R5)</f>
         <v>1.5</v>
       </c>
@@ -1803,7 +2185,7 @@
       <c r="Q7" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="R7" s="14">
+      <c r="R7" s="10">
         <f>MIN(R6,B6)</f>
         <v>1.5</v>
       </c>
@@ -1973,7 +2355,7 @@
       <c r="K12" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="L12" s="13">
+      <c r="L12" s="9">
         <f>POWER(L21*POWER(B12,3)/(6*L19),0.5)</f>
         <v>7.0561909348085647</v>
       </c>
@@ -1990,11 +2372,11 @@
       <c r="S12" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="U12" s="7" t="s">
+      <c r="U12" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="V12" s="7"/>
-      <c r="W12" s="7"/>
+      <c r="V12" s="19"/>
+      <c r="W12" s="19"/>
     </row>
     <row r="13" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
@@ -2006,11 +2388,11 @@
       <c r="C13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K13" s="10" t="s">
+      <c r="K13" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="L13" s="11"/>
-      <c r="M13" s="12"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="14"/>
       <c r="Q13" s="4" t="s">
         <v>78</v>
       </c>
@@ -2021,9 +2403,9 @@
       <c r="S13" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="U13" s="7"/>
-      <c r="V13" s="7"/>
-      <c r="W13" s="7"/>
+      <c r="U13" s="19"/>
+      <c r="V13" s="19"/>
+      <c r="W13" s="19"/>
     </row>
     <row r="14" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
@@ -2053,7 +2435,7 @@
         <v>safe</v>
       </c>
       <c r="S14" s="3"/>
-      <c r="U14" s="8" t="s">
+      <c r="U14" s="7" t="s">
         <v>56</v>
       </c>
       <c r="V14" s="2">
@@ -2136,14 +2518,14 @@
         <v>29</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>60</v>
+        <v>97</v>
       </c>
       <c r="V16" s="2">
-        <f>(B3-2)*2</f>
-        <v>84</v>
+        <f>(MAX(R3,R17)-R17)*2*R17*B19*2+B22*2*(MAX(R21,R35)-R35)*R35</f>
+        <v>35.34018900861259</v>
       </c>
       <c r="W16" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2166,15 +2548,24 @@
       <c r="M17" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="Q17" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="R17" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="S17" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="U17" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="V17" s="2">
-        <f>B9/(V15*B17 + V16*B18)</f>
-        <v>1.0056818181818181</v>
+        <f>(B3-2)*2</f>
+        <v>84</v>
       </c>
       <c r="W17" s="3" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2187,20 +2578,20 @@
       <c r="C18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K18" s="10" t="s">
+      <c r="K18" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="L18" s="11"/>
-      <c r="M18" s="12"/>
-      <c r="U18" s="4" t="s">
-        <v>64</v>
+      <c r="L18" s="13"/>
+      <c r="M18" s="14"/>
+      <c r="U18" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="V18" s="2">
-        <f>B10/(V15*B17 + V16*B18)</f>
-        <v>2.2727272727272728E-2</v>
+        <f>B9/(V15*B17 + V17*B18 + V16)</f>
+        <v>0.83751226319186667</v>
       </c>
       <c r="W18" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2223,20 +2614,20 @@
       <c r="M19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="Q19" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="R19" s="22"/>
-      <c r="S19" s="23"/>
+      <c r="Q19" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="R19" s="21"/>
+      <c r="S19" s="22"/>
       <c r="U19" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="V19" s="2">
-        <f>POWER(POWER(V17,2) +3*POWER(V18,2),0.5)</f>
-        <v>1.0064519393385594</v>
+        <f>B10/(V15*B17 + V17*B18 + V16)</f>
+        <v>1.8926830806595858E-2</v>
       </c>
       <c r="W19" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2246,37 +2637,39 @@
       <c r="B20" s="5">
         <v>1.5</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="11" t="s">
         <v>15</v>
       </c>
       <c r="K20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L20" s="9" t="str">
+      <c r="L20" s="8" t="str">
         <f>IF(L19*1000 &lt; B11, "safe", "unsafe")</f>
         <v>safe</v>
       </c>
       <c r="M20" s="3"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="19"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="24"/>
       <c r="S20" s="25"/>
-      <c r="U20" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="V20" s="2" t="str">
-        <f>IF(AND(MAX(V17:V18) &lt; V14, V19 &lt; V14*1.1), "safe", "unsafe")</f>
-        <v>safe</v>
-      </c>
-      <c r="W20" s="3"/>
-    </row>
-    <row r="21" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="U20" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="V20" s="2">
+        <f>POWER(POWER(V18,2) +3*POWER(V19,2),0.5)</f>
+        <v>0.83815360511657233</v>
+      </c>
+      <c r="W20" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>86</v>
       </c>
       <c r="B21" s="5">
         <v>20</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="11" t="s">
         <v>15</v>
       </c>
       <c r="K21" s="4" t="s">
@@ -2290,15 +2683,23 @@
         <v>18</v>
       </c>
       <c r="Q21" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="R21" s="13" t="str">
+        <v>99</v>
+      </c>
+      <c r="R21" s="9" t="str">
         <f>IF((B8-B5)/2 - L12 &gt; 0, (B8-B5)/2 - L12, "no stiffeners required")</f>
         <v>no stiffeners required</v>
       </c>
       <c r="S21" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="U21" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="V21" s="2" t="str">
+        <f>IF(AND(MAX(V18:V19) &lt; V14, V20 &lt; V14*1.1), "safe", "unsafe")</f>
+        <v>safe</v>
+      </c>
+      <c r="W21" s="3"/>
     </row>
     <row r="22" spans="1:23" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
@@ -2323,7 +2724,7 @@
       <c r="Q22" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="R22" s="13">
+      <c r="R22" s="9">
         <f>IF(B22&gt;0, IF(B24, B24, _xlfn.CEILING.MATH(L3/3)), 0)</f>
         <v>0</v>
       </c>
@@ -2338,7 +2739,7 @@
       <c r="B23" s="5">
         <v>2</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="11" t="s">
         <v>15</v>
       </c>
       <c r="K23" s="4" t="s">
@@ -2369,7 +2770,7 @@
       <c r="B24" s="5">
         <v>16</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="11" t="s">
         <v>15</v>
       </c>
       <c r="K24" s="4" t="s">
@@ -2385,7 +2786,7 @@
       <c r="Q24" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="R24" s="13">
+      <c r="R24" s="9">
         <f>MAX(B23,R23)</f>
         <v>2</v>
       </c>
@@ -2407,7 +2808,7 @@
       <c r="Q25" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="R25" s="14">
+      <c r="R25" s="10">
         <f>MIN(R24,B6)</f>
         <v>2</v>
       </c>
@@ -2549,107 +2950,118 @@
         <v>29</v>
       </c>
     </row>
+    <row r="35" spans="17:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="Q35" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="R35" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="S35" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="Q19:S20"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="K1:M2"/>
+    <mergeCell ref="U1:W2"/>
+    <mergeCell ref="U12:W13"/>
     <mergeCell ref="K18:M18"/>
     <mergeCell ref="K13:M13"/>
     <mergeCell ref="F1:H2"/>
     <mergeCell ref="K8:M8"/>
     <mergeCell ref="Q1:S2"/>
-    <mergeCell ref="Q19:S20"/>
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="K1:M2"/>
-    <mergeCell ref="U1:W2"/>
-    <mergeCell ref="U12:W13"/>
   </mergeCells>
   <conditionalFormatting sqref="V7:V9">
-    <cfRule type="cellIs" dxfId="21" priority="28" operator="lessThan">
+    <cfRule type="cellIs" dxfId="57" priority="34" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="29" operator="lessThan">
+    <cfRule type="cellIs" dxfId="56" priority="35" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L28">
-    <cfRule type="cellIs" dxfId="19" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="36" operator="equal">
       <formula>"unsafe"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="36" operator="equal">
       <formula>"safe"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V9">
-    <cfRule type="cellIs" dxfId="17" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="28" operator="equal">
       <formula>"unsafe"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="23" operator="equal">
-      <formula>"safe"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V18:V19">
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="17" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V19">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
-      <formula>"unsafe"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
-      <formula>"safe"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V20">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
-      <formula>"unsafe"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="29" operator="equal">
       <formula>"safe"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="16" operator="equal">
       <formula>"unsafe"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="17" operator="equal">
       <formula>"safe"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="43" priority="14" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="42" priority="15" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R14">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="12" operator="equal">
       <formula>"safe"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="13" operator="equal">
       <formula>"unsafe"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="cellIs" dxfId="3" priority="31" operator="lessThan">
+    <cfRule type="cellIs" dxfId="39" priority="37" operator="lessThan">
       <formula>$R$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R32">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="9" operator="equal">
       <formula>"safe"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="10" operator="equal">
       <formula>"unsafe"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="36" priority="7" operator="lessThan">
       <formula>$R$23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V19:V20">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V20">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+      <formula>"unsafe"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+      <formula>"safe"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V21">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"unsafe"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"safe"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>